<commit_message>
added ddt and screenshot for checkout test case 5 6 7
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26107D57-83B8-496C-8845-348F97502C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EB00F6-35F2-453C-8115-E56159E78441}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="1710" windowWidth="14400" windowHeight="7730" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="3370" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Costabirfernandeserrolcostabirmenezesdsouzacabralsouzapereira</t>
+  </si>
+  <si>
+    <t>demo4@example.com</t>
+  </si>
+  <si>
+    <t>test1234</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,6 +544,30 @@
       </c>
       <c r="B6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added failing tc for login, updated codes for checkout(01,001 to 007) and login(001 to 008) ----> All working
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689613F4-6CF5-476F-BF19-19F8F1CF39A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC484E3A-5351-47E9-A855-583E00B2C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="790" yWindow="2050" windowWidth="14400" windowHeight="7730" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>TESTER123</t>
   </si>
 </sst>
 </file>
@@ -491,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,12 +573,21 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{7368AE4C-B007-45E9-822F-BFB8A7959340}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{D3715D07-8D3F-4638-AF3A-87ABAC2CC153}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{4F448A56-0DE0-4E38-9DFA-83671F9FBE13}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{3B82F7CA-1993-4737-8D3A-D7AB65DF1F9C}"/>
+    <hyperlink ref="A10" r:id="rId5" xr:uid="{AC1B3D0A-6342-43EC-84D2-DAC122A8C522}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -585,7 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D98C79-261C-4370-99A6-A1E78EFA5559}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
used single ddt and added screenshot with extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC484E3A-5351-47E9-A855-583E00B2C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC78EAD-5C27-46E9-B653-F97DD11DA8E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="790" yWindow="2050" windowWidth="14400" windowHeight="7730" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Checkout" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact" sheetId="3" r:id="rId3"/>
+    <sheet name="Registration" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>Username</t>
   </si>
@@ -119,13 +121,97 @@
   </si>
   <si>
     <t>TESTER123</t>
+  </si>
+  <si>
+    <t>demo@email.com</t>
+  </si>
+  <si>
+    <t>Testing if this field is working without</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>demo1@example</t>
+  </si>
+  <si>
+    <t>When will the iPad Air be in stock again</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>demo1@example.com</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Errol5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>demo2@example.com</t>
+  </si>
+  <si>
+    <t>demo3@example.com</t>
+  </si>
+  <si>
+    <t>demo5@example.com</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>Raunak</t>
+  </si>
+  <si>
+    <t>Naik</t>
+  </si>
+  <si>
+    <t>testing@example.com</t>
+  </si>
+  <si>
+    <t>testing123</t>
+  </si>
+  <si>
+    <t>test4567</t>
+  </si>
+  <si>
+    <t>testing1@example.com</t>
+  </si>
+  <si>
+    <t>testing2@example.com</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Raunakabcdefghijklmnopqrstuvwxyza</t>
+  </si>
+  <si>
+    <t>testing3@example.com</t>
+  </si>
+  <si>
+    <t>Naikabcdefghijklmnopqrstuvwxyzabc</t>
+  </si>
+  <si>
+    <t>testing4@example.com</t>
+  </si>
+  <si>
+    <t>testing5@example.com</t>
+  </si>
+  <si>
+    <t>22222222222222222222222222222222222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +229,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,10 +268,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,4 +818,332 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158A9D05-E6E3-48FF-BB36-45C246B8D648}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{122097EE-9CB1-45A0-A842-DC3AAE0622CE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C20B527A-3181-4869-B48F-D5F98B2F74AB}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{59FD2F43-A9CF-4338-93DA-AEF2F08A1057}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{4CDA185E-14FA-477C-A33D-8E43C5C0D8B1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1">
+        <v>12345</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>122345</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3">
+        <v>123455</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>12345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{292274E7-A874-44D1-9B4D-EC8374E42B76}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{8F9D6AB1-D00F-4D29-82EE-54A2BBBE4D10}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the end test case
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC484E3A-5351-47E9-A855-583E00B2C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738F82A6-99E7-41E7-8FA8-D111B150F12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="790" yWindow="2050" windowWidth="14400" windowHeight="7730" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>TESTER123</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,6 +582,14 @@
       </c>
       <c r="B10" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Search sheet and Wishlist sheet in LoginDDT.xlsl
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746027E-1EF7-46D8-A3B5-6BF436EAC56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CF7A6D-BCC3-4DF0-8464-5D70800C4708}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11265" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Checkout" sheetId="2" r:id="rId2"/>
     <sheet name="Contact" sheetId="3" r:id="rId3"/>
     <sheet name="Wishlist" sheetId="5" r:id="rId4"/>
-    <sheet name="Registration" sheetId="4" r:id="rId5"/>
+    <sheet name="Search" sheetId="6" r:id="rId5"/>
+    <sheet name="Registration" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>Username</t>
   </si>
@@ -212,13 +213,79 @@
   </si>
   <si>
     <t>Shriya@123</t>
+  </si>
+  <si>
+    <t>Search Query</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>iPhone is a revolutionary new mobile phone that allows you to make a call by simply tapping a name o..</t>
+  </si>
+  <si>
+    <t>$123.20</t>
+  </si>
+  <si>
+    <t>IPHONE</t>
+  </si>
+  <si>
+    <t>iMac</t>
+  </si>
+  <si>
+    <t>Just when you thought iMac had everything, now there´s even more. More powerful Intel Core 2 Duo pro..</t>
+  </si>
+  <si>
+    <t>$122.00</t>
+  </si>
+  <si>
+    <t>mac</t>
+  </si>
+  <si>
+    <t>MacBook</t>
+  </si>
+  <si>
+    <t>Intel Core 2 Duo processor Powered by an Intel Core 2 Duo processor at speeds up to 2.16GHz, t..</t>
+  </si>
+  <si>
+    <t>$602.00</t>
+  </si>
+  <si>
+    <t>asjdnjasndjbnajsdbjadbjasbndjasbnjdbn</t>
+  </si>
+  <si>
+    <t>MacBook Air</t>
+  </si>
+  <si>
+    <t>MacBook Air is ultrathin, ultraportable, and ultra unlike anything else. But you don’t lose in..</t>
+  </si>
+  <si>
+    <t>$1,202.00</t>
+  </si>
+  <si>
+    <t>MacBook Pro</t>
+  </si>
+  <si>
+    <t>Latest Intel mobile architecture Powered by the most advanced mobile processors from Intel, ..</t>
+  </si>
+  <si>
+    <t>$2,000.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +310,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,12 +350,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,13 +679,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.90625" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -616,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -624,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -632,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -640,10 +717,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -651,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -659,7 +736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -667,7 +744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -675,7 +752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -703,13 +780,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.36328125" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -732,7 +809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -752,7 +829,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -775,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -798,7 +875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -835,9 +912,9 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -848,7 +925,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -859,7 +936,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -870,7 +947,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -896,13 +973,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C39830-CC58-4AA0-8F8D-7E0A93994147}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -928,6 +1005,108 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9F7286-F605-4316-9E67-E214F22C79C5}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -935,9 +1114,9 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -957,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -977,7 +1156,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -994,7 +1173,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1014,7 +1193,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1034,7 +1213,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -1054,7 +1233,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1074,7 +1253,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>43</v>
@@ -1092,7 +1271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1112,7 +1291,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1132,7 +1311,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -1152,7 +1331,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Updated end test case
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB85A3B-D81C-467A-A123-DB2C5BA55120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C307831F-48C8-4E72-8D29-36369DF53034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>TESTER123</t>
+  </si>
+  <si>
+    <t>tony@starkenterprises.com</t>
+  </si>
+  <si>
+    <t>ironman</t>
   </si>
 </sst>
 </file>
@@ -494,9 +500,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -579,6 +585,14 @@
       </c>
       <c r="B10" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated end test case class
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6638966-7AAE-433E-9EA3-E27A63B937FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746027E-1EF7-46D8-A3B5-6BF436EAC56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Checkout" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact" sheetId="3" r:id="rId3"/>
+    <sheet name="Wishlist" sheetId="5" r:id="rId4"/>
+    <sheet name="Registration" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -46,13 +49,22 @@
     <t>tester1@gmail.com</t>
   </si>
   <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>tester@gmail.com</t>
+  </si>
+  <si>
     <t>tester123</t>
   </si>
   <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>tester@gmail.com</t>
+    <t>demo4@example.com</t>
+  </si>
+  <si>
+    <t>test1234</t>
+  </si>
+  <si>
+    <t>TESTER123</t>
   </si>
   <si>
     <t>FirstName</t>
@@ -61,6 +73,9 @@
     <t>LastName</t>
   </si>
   <si>
+    <t>Address1</t>
+  </si>
+  <si>
     <t>City</t>
   </si>
   <si>
@@ -76,27 +91,24 @@
     <t>Diffa</t>
   </si>
   <si>
+    <t>H.No 493, Somewhere, Some Place</t>
+  </si>
+  <si>
+    <t>Somewhere</t>
+  </si>
+  <si>
+    <t>A2345</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
     <t>Pinto</t>
   </si>
   <si>
-    <t>H.No 493, Somewhere, Some Place</t>
-  </si>
-  <si>
-    <t>Somewhere</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>Address1</t>
-  </si>
-  <si>
-    <t>A2345</t>
-  </si>
-  <si>
     <t>Errol</t>
   </si>
   <si>
@@ -112,26 +124,101 @@
     <t>Costabirfernandeserrolcostabirmenezesdsouzacabralsouzapereira</t>
   </si>
   <si>
-    <t>demo4@example.com</t>
-  </si>
-  <si>
-    <t>test1234</t>
-  </si>
-  <si>
-    <t>TESTER123</t>
-  </si>
-  <si>
-    <t>tony@starkenterprises.com</t>
-  </si>
-  <si>
-    <t>ironman</t>
+    <t>demo@email.com</t>
+  </si>
+  <si>
+    <t>Testing if this field is working without</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>demo1@example</t>
+  </si>
+  <si>
+    <t>When will the iPad Air be in stock again</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>demo1@example.com</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>Shriya@123</t>
+  </si>
+  <si>
+    <t>Errol5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>demo2@example.com</t>
+  </si>
+  <si>
+    <t>demo3@example.com</t>
+  </si>
+  <si>
+    <t>demo5@example.com</t>
+  </si>
+  <si>
+    <t>abcdefg</t>
+  </si>
+  <si>
+    <t>Raunak</t>
+  </si>
+  <si>
+    <t>Naik</t>
+  </si>
+  <si>
+    <t>testing@example.com</t>
+  </si>
+  <si>
+    <t>testing123</t>
+  </si>
+  <si>
+    <t>test4567</t>
+  </si>
+  <si>
+    <t>testing1@example.com</t>
+  </si>
+  <si>
+    <t>testing2@example.com</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Raunakabcdefghijklmnopqrstuvwxyza</t>
+  </si>
+  <si>
+    <t>testing3@example.com</t>
+  </si>
+  <si>
+    <t>Naikabcdefghijklmnopqrstuvwxyzabc</t>
+  </si>
+  <si>
+    <t>testing4@example.com</t>
+  </si>
+  <si>
+    <t>testing5@example.com</t>
+  </si>
+  <si>
+    <t>22222222222222222222222222222222222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +236,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,10 +275,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -500,19 +596,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,79 +616,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -615,126 +703,489 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="63.36328125" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158A9D05-E6E3-48FF-BB36-45C246B8D648}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{122097EE-9CB1-45A0-A842-DC3AAE0622CE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C20B527A-3181-4869-B48F-D5F98B2F74AB}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{59FD2F43-A9CF-4338-93DA-AEF2F08A1057}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{4CDA185E-14FA-477C-A33D-8E43C5C0D8B1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C39830-CC58-4AA0-8F8D-7E0A93994147}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{FE0D3390-4641-4A36-9409-12C71F811A6C}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{150F1A6D-450E-4746-9B66-20A69ADE46B6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1">
+        <v>12345</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>122345</v>
+      </c>
+      <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3">
+        <v>123455</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>12345</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2123434565</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{292274E7-A874-44D1-9B4D-EC8374E42B76}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{8F9D6AB1-D00F-4D29-82EE-54A2BBBE4D10}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checkout and Login ---> Ready
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\Desktop\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7746027E-1EF7-46D8-A3B5-6BF436EAC56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53212D5-DA52-477D-BB66-CDC1145C1DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="59">
   <si>
     <t>Username</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Shriya@123</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C39830-CC58-4AA0-8F8D-7E0A93994147}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -931,11 +934,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -959,16 +965,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D2">
-        <v>122345</v>
+        <v>2123434565</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -979,19 +985,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D3">
-        <v>123455</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
+        <v>2123434565</v>
+      </c>
+      <c r="E3">
+        <v>12345678</v>
+      </c>
+      <c r="F3">
+        <v>12345678</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1175,16 +1181,16 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" xr:uid="{292274E7-A874-44D1-9B4D-EC8374E42B76}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{8F9D6AB1-D00F-4D29-82EE-54A2BBBE4D10}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
+    <hyperlink ref="C2" r:id="rId10" xr:uid="{BC862966-ECEA-41E5-9862-97F09A338BBA}"/>
+    <hyperlink ref="C3" r:id="rId11" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed logout and forgot password test case file
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1D231F-9657-485A-B22D-AB9B77AA3881}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C084FB-ACCE-4458-8EF0-40607B52FC9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11265" activeTab="5" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11265" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
   <si>
     <t>Username</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>$2,000.00</t>
+  </si>
+  <si>
+    <t>xyz-123@yahoo.com</t>
+  </si>
+  <si>
+    <t>deekshavishwakarma@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -682,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,6 +775,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{7368AE4C-B007-45E9-822F-BFB8A7959340}"/>
@@ -776,6 +796,8 @@
     <hyperlink ref="A3" r:id="rId3" xr:uid="{4F448A56-0DE0-4E38-9DFA-83671F9FBE13}"/>
     <hyperlink ref="A4" r:id="rId4" xr:uid="{3B82F7CA-1993-4737-8D3A-D7AB65DF1F9C}"/>
     <hyperlink ref="A10" r:id="rId5" xr:uid="{AC1B3D0A-6342-43EC-84D2-DAC122A8C522}"/>
+    <hyperlink ref="A11" r:id="rId6" display="mailto:xyz-123@yahoo.com" xr:uid="{342E5E48-DB91-4156-82FE-8791A0E78056}"/>
+    <hyperlink ref="A12" r:id="rId7" display="mailto:deekshavishwakarma@yahoo.com" xr:uid="{992A7970-FDBC-46D1-BF22-815F78CB6C49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1283,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710768C2-E9F9-4857-8660-8051F2581FDE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor changes with excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C084FB-ACCE-4458-8EF0-40607B52FC9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495CFB54-0BB0-45BB-8BCD-4284D475CC03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11265" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11265" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
   <si>
     <t>Username</t>
   </si>
@@ -294,13 +294,16 @@
   </si>
   <si>
     <t>deekshavishwakarma@yahoo.com</t>
+  </si>
+  <si>
+    <t>demo@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +340,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -365,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -373,6 +382,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -690,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1037,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,24 +1115,24 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4">
-        <v>123</v>
+        <v>36</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>123</v>
+        <v>2123434565</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1283,21 +1293,43 @@
         <v>45</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" xr:uid="{292274E7-A874-44D1-9B4D-EC8374E42B76}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
-    <hyperlink ref="C12" r:id="rId9" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
-    <hyperlink ref="C2" r:id="rId10" xr:uid="{BC862966-ECEA-41E5-9862-97F09A338BBA}"/>
-    <hyperlink ref="C3" r:id="rId11" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{18ACA63D-D94F-4BDF-89C4-BAE41EE3D548}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{7DD0123C-A89E-474C-8E8E-EC930CC345A0}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{99F0B7E9-9716-4CF8-BBD5-6F1F5F6BC552}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{7AE90970-5EF0-45BD-B9D7-53623853E903}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{E9633283-3F02-4103-B93D-4D52559DAC22}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{F83A6761-0081-43B9-B0F6-C7F6375E07C3}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{AE79FAE5-4AEA-4A47-AE26-5FCE3033917D}"/>
+    <hyperlink ref="C2" r:id="rId9" xr:uid="{BC862966-ECEA-41E5-9862-97F09A338BBA}"/>
+    <hyperlink ref="C3" r:id="rId10" xr:uid="{758F9935-D65C-4659-B1AC-8857DAD79D84}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{3B3F03B5-598E-4B4B-B8AB-EE32DA1FDF4A}"/>
+    <hyperlink ref="C4" r:id="rId12" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
made minor chnages to loginDDT
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495CFB54-0BB0-45BB-8BCD-4284D475CC03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DDE9D4-EF3B-4C4C-8B4F-8808FFEB614A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11265" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
   <si>
     <t>Username</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>demo@example.com</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -701,16 +704,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -718,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -726,7 +729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -734,7 +737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -742,10 +745,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -753,7 +756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -761,7 +764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -769,7 +772,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -777,7 +780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -785,13 +788,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -821,13 +824,13 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="63.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.453125" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -850,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -870,7 +873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -893,7 +896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -916,7 +919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -953,9 +956,9 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -966,7 +969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -977,7 +980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -988,7 +991,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1018,9 +1021,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -1050,15 +1053,15 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1091,14 +1094,14 @@
       <c r="D2">
         <v>2123434565</v>
       </c>
-      <c r="E2">
-        <v>123</v>
-      </c>
-      <c r="F2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1155,7 +1158,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>42</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>43</v>
@@ -1213,7 +1216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1329,7 +1332,7 @@
     <hyperlink ref="C4" r:id="rId12" xr:uid="{A25663FA-A139-4B93-AB19-9C9E90421C45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1341,15 +1344,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1366,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Minor changes to LoginDDT
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maven Project\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DDE9D4-EF3B-4C4C-8B4F-8808FFEB614A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0531FF-E4EC-4529-9C32-00C6AABF73B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Contact" sheetId="3" r:id="rId3"/>
     <sheet name="Wishlist" sheetId="5" r:id="rId4"/>
     <sheet name="Registration" sheetId="4" r:id="rId5"/>
-    <sheet name="Search" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Search" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
   <si>
     <t>Username</t>
   </si>
@@ -300,6 +301,54 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>eu fugiat nulla pariatur</t>
+  </si>
+  <si>
+    <t>elit</t>
+  </si>
+  <si>
+    <t>in voluptate velit esse cillum dolore</t>
+  </si>
+  <si>
+    <t>adipiscing</t>
+  </si>
+  <si>
+    <t>laboris nisi ut aliquip ex ea commodo consequat</t>
+  </si>
+  <si>
+    <t>consectetur</t>
+  </si>
+  <si>
+    <t>quis nostrud exercitation ullamco</t>
+  </si>
+  <si>
+    <t>amet</t>
+  </si>
+  <si>
+    <t>Ut enim ad minim veniam</t>
+  </si>
+  <si>
+    <t>sit</t>
+  </si>
+  <si>
+    <t>sed do eiusmod tempor incididunt ut labore et dolore magna aliqua</t>
+  </si>
+  <si>
+    <t>dolor</t>
+  </si>
+  <si>
+    <t>consectetur adipiscing elit</t>
+  </si>
+  <si>
+    <t>ipsum</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet</t>
+  </si>
+  <si>
+    <t>lorem</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1337,6 +1386,85 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF384E3E-8CDD-4EA3-802F-BD2E81EAFACF}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710768C2-E9F9-4857-8660-8051F2581FDE}">
   <dimension ref="A1:D6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Minor changes in ContactUs.java
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0531FF-E4EC-4529-9C32-00C6AABF73B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BAE3EF-B616-42D1-A229-11AB4D842170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Contact" sheetId="3" r:id="rId3"/>
     <sheet name="Wishlist" sheetId="5" r:id="rId4"/>
     <sheet name="Registration" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Apple Cinema" sheetId="7" r:id="rId6"/>
     <sheet name="Search" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="103">
   <si>
     <t>Username</t>
   </si>
@@ -999,10 +999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158A9D05-E6E3-48FF-BB36-45C246B8D648}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1049,6 +1049,17 @@
       </c>
       <c r="C4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF384E3E-8CDD-4EA3-802F-BD2E81EAFACF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added searchQuery DDT functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BAE3EF-B616-42D1-A229-11AB4D842170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F1E65-1103-4F51-BB7E-5DE495C1E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Checkout" sheetId="2" r:id="rId2"/>
     <sheet name="Contact" sheetId="3" r:id="rId3"/>
-    <sheet name="Wishlist" sheetId="5" r:id="rId4"/>
-    <sheet name="Registration" sheetId="4" r:id="rId5"/>
-    <sheet name="Apple Cinema" sheetId="7" r:id="rId6"/>
-    <sheet name="Search" sheetId="6" r:id="rId7"/>
+    <sheet name="search queries" sheetId="8" r:id="rId4"/>
+    <sheet name="Wishlist" sheetId="5" r:id="rId5"/>
+    <sheet name="Registration" sheetId="4" r:id="rId6"/>
+    <sheet name="Apple Cinema" sheetId="7" r:id="rId7"/>
+    <sheet name="Search" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>Username</t>
   </si>
@@ -349,6 +350,12 @@
   </si>
   <si>
     <t>lorem</t>
+  </si>
+  <si>
+    <t>macbook</t>
+  </si>
+  <si>
+    <t>iphone</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{158A9D05-E6E3-48FF-BB36-45C246B8D648}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1074,6 +1081,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CC5CFD-0613-466C-8881-9ABAE84A95A0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C39830-CC58-4AA0-8F8D-7E0A93994147}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1108,7 +1140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -1396,7 +1428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF384E3E-8CDD-4EA3-802F-BD2E81EAFACF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1475,7 +1507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710768C2-E9F9-4857-8660-8051F2581FDE}">
   <dimension ref="A1:D6"/>
   <sheetViews>

</xml_diff>

<commit_message>
All testing changes done except for Reg, Search and Wishlist
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diffa_pinto\eclipse-workspace-new\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F1E65-1103-4F51-BB7E-5DE495C1E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55127E27-4C5F-4D20-B30D-3969A4204057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Registration" sheetId="4" r:id="rId6"/>
     <sheet name="Apple Cinema" sheetId="7" r:id="rId7"/>
     <sheet name="Search" sheetId="6" r:id="rId8"/>
+    <sheet name="Coupon Codes and Quantity" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
   <si>
     <t>Username</t>
   </si>
@@ -301,9 +302,6 @@
     <t>demo@example.com</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>eu fugiat nulla pariatur</t>
   </si>
   <si>
@@ -356,6 +354,27 @@
   </si>
   <si>
     <t>iphone</t>
+  </si>
+  <si>
+    <t>tester234@gmail.com</t>
+  </si>
+  <si>
+    <t>tester2@gmail.com</t>
+  </si>
+  <si>
+    <t>Coupon Codes</t>
+  </si>
+  <si>
+    <t>15Off</t>
+  </si>
+  <si>
+    <t>tester234</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -757,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -795,7 +814,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -857,6 +876,17 @@
       <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -867,6 +897,7 @@
     <hyperlink ref="A10" r:id="rId5" xr:uid="{AC1B3D0A-6342-43EC-84D2-DAC122A8C522}"/>
     <hyperlink ref="A11" r:id="rId6" display="mailto:xyz-123@yahoo.com" xr:uid="{342E5E48-DB91-4156-82FE-8791A0E78056}"/>
     <hyperlink ref="A12" r:id="rId7" display="mailto:deekshavishwakarma@yahoo.com" xr:uid="{992A7970-FDBC-46D1-BF22-815F78CB6C49}"/>
+    <hyperlink ref="A13" r:id="rId8" xr:uid="{266F58E8-C2D2-499E-8598-22FEEFF5FB58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1009,7 +1040,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1084,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CC5CFD-0613-466C-8881-9ABAE84A95A0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1092,12 +1123,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1144,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DD2B35-7E4B-4369-86CE-A4A31F46A307}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1187,10 +1218,10 @@
         <v>2123434565</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1433,73 +1464,76 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="58.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1608,4 +1642,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AEC692-0A65-4085-9CEF-E5B89B9C79F2}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ddt functionality in some classes
</commit_message>
<xml_diff>
--- a/src/test/resources/loginDDT.xlsx
+++ b/src/test/resources/loginDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini Project Maven\PSLMiniProject\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916F1E65-1103-4F51-BB7E-5DE495C1E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BA2CB8-46F7-426E-9374-922C5CCE09AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FC8C67C2-FED1-41A8-80E0-D2B7FD42E917}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3115BA-B098-4BA6-A8EF-454B33089B2C}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1084,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CC5CFD-0613-466C-8881-9ABAE84A95A0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1150,6 +1150,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
     <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>